<commit_message>
added my hours of work
</commit_message>
<xml_diff>
--- a/06_weitere_Dateien/Arbeitsverteilung.xlsx
+++ b/06_weitere_Dateien/Arbeitsverteilung.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -82,16 +85,57 @@
   </si>
   <si>
     <t>Erstellung meines Teils der PowerPoint Präsenatation</t>
+  </si>
+  <si>
+    <t>Erstellung der Teile des Berichts, die mit meinem Kürzel CD gekennzeichnet sind</t>
+  </si>
+  <si>
+    <t>Erstellung der Teile der Dokumentation, die mit meinem Kürzel CD gekennzeichnet sind</t>
+  </si>
+  <si>
+    <t>Erstellung meines Teils der PowerPoint Präsentation</t>
+  </si>
+  <si>
+    <t>JavaScript-Code für Projekt schreiben (App starten, Login-Daten eintragen, Passende Note anhand des Namens suchen, Buttons automatisiert klicken, Noten beim Studenten eintragen)</t>
+  </si>
+  <si>
+    <t>Projekt aufgesetzt (Electron installiert)</t>
+  </si>
+  <si>
+    <t>Excel-Vorlagen erstellen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,16 +158,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -182,7 +254,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -217,7 +289,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -394,7 +466,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,21 +474,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -430,7 +502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -438,81 +510,154 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
-      <c r="B4" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="42">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+    <row r="13" spans="1:4">
+      <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
+    <row r="14" spans="1:4">
+      <c r="C14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+    <row r="15" spans="1:4">
+      <c r="C15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
+    <row r="16" spans="1:4">
+      <c r="C16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
+    <row r="20" spans="3:3">
+      <c r="C20" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B3:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
einzeleinträge marco hinzugefügt bis zum aktuellen stand
</commit_message>
<xml_diff>
--- a/06_weitere_Dateien/Arbeitsverteilung.xlsx
+++ b/06_weitere_Dateien/Arbeitsverteilung.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8571142A-3B24-4B3D-8E0D-9E2BE681EFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -103,13 +104,40 @@
   </si>
   <si>
     <t>Excel-Vorlagen erstellen</t>
+  </si>
+  <si>
+    <t>Erstellung meines Teils der PowerPoint Präsentation und das Zusammenfügen und erstellen des Designs der PowerPoint der Gruppe</t>
+  </si>
+  <si>
+    <t>Erstellung des Berichts gekennzeichnet mit dem Kürzel MS</t>
+  </si>
+  <si>
+    <t>Adobe XD Mock-Up</t>
+  </si>
+  <si>
+    <t>Erstellung der Master CSS</t>
+  </si>
+  <si>
+    <t>Erstellung HTML Dateien für Sprint 2 Review inkl neuem CSS</t>
+  </si>
+  <si>
+    <t>Eintrag am 13.5</t>
+  </si>
+  <si>
+    <t>Erstellung des Logos</t>
+  </si>
+  <si>
+    <t>Style-Tile inkl. Schriftrecherche</t>
+  </si>
+  <si>
+    <t>Nacharbeiten an HTML Seiten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +164,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,7 +207,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,14 +216,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -466,29 +506,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -502,17 +542,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
@@ -522,9 +562,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
@@ -532,9 +572,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>26</v>
       </c>
@@ -542,9 +582,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
@@ -552,9 +592,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
@@ -562,9 +602,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -572,9 +612,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>23</v>
       </c>
@@ -582,68 +622,137 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="C13" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="C14" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="C15" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="C16" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
-      <c r="C17" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="3:3">
-      <c r="C18" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:3">
-      <c r="C19" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
-      <c r="C20" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>20</v>
       </c>
     </row>
@@ -652,6 +761,7 @@
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B3:B9"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
updated my work amount
</commit_message>
<xml_diff>
--- a/06_weitere_Dateien/Arbeitsverteilung.xlsx
+++ b/06_weitere_Dateien/Arbeitsverteilung.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55BA522-E67C-4A7A-B0A5-19A2BFBC5DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -128,12 +127,15 @@
   </si>
   <si>
     <t>Nacharbeiten an HTML Seiten</t>
+  </si>
+  <si>
+    <t>Abklärung zur Aufnahme vom Video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,8 +191,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -220,19 +224,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+  <cellStyles count="15">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,29 +509,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -539,7 +545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -547,7 +553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>3</v>
@@ -559,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="2" t="s">
@@ -569,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
@@ -579,7 +585,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="2" t="s">
@@ -589,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="42">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
@@ -599,7 +605,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
@@ -609,7 +615,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
@@ -619,144 +625,154 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="5"/>
-      <c r="B10" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1"/>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
+      <c r="C18" t="s">
         <v>34</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="21" spans="1:4">
+      <c r="C21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="22" spans="1:4">
+      <c r="C22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="23" spans="1:4">
+      <c r="C23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+    <row r="24" spans="1:4">
+      <c r="C24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="25" spans="1:4">
+      <c r="C25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="26" spans="1:4">
+      <c r="C26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+    <row r="27" spans="1:4">
+      <c r="C27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="28" spans="1:4">
+      <c r="C28" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B3:B10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added jonas' document and the combination of both
</commit_message>
<xml_diff>
--- a/06_weitere_Dateien/Arbeitsverteilung.xlsx
+++ b/06_weitere_Dateien/Arbeitsverteilung.xlsx
@@ -509,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -520,7 +520,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -572,7 +572,7 @@
         <v>22</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>